<commit_message>
openmp raw data added and also in excel
All data is in, and a graph can be made from the openmp sheet in the excel file
</commit_message>
<xml_diff>
--- a/proj4_data.xlsx
+++ b/proj4_data.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10723"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmac2\Documents\CIS 520\proj4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/SeniorYear/SecondSemester/OperatingSystems/proj4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C0B765-88BC-4414-8B11-643AC9DF3FC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C417F961-D22C-9E44-8E3A-4E83E3661024}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E93CB639-010A-410E-81EE-401D241EC0E8}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{E93CB639-010A-410E-81EE-401D241EC0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="openmp" sheetId="2" r:id="rId2"/>
+    <sheet name="pthreads" sheetId="3" r:id="rId3"/>
+    <sheet name="mpi" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="24">
   <si>
     <t>MPI</t>
   </si>
@@ -87,12 +88,30 @@
   <si>
     <t xml:space="preserve">This implementation was discarded due to poor performance. </t>
   </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Miliseconds</t>
+  </si>
+  <si>
+    <t>Problem Size: 100K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +141,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -155,13 +188,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -480,32 +515,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1049F09C-3447-4F8C-B499-E90E3A98F0EC}">
   <dimension ref="A1:AJ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.61328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.3828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.765625" customWidth="1"/>
-    <col min="8" max="8" width="9.53515625" customWidth="1"/>
-    <col min="9" max="9" width="6.3828125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.07421875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.15234375" customWidth="1"/>
-    <col min="14" max="14" width="9.23046875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="17.07421875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -537,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -574,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -593,7 +628,7 @@
         <v>93130</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -612,7 +647,7 @@
         <v>278837</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -631,7 +666,7 @@
         <v>1118151</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -650,7 +685,7 @@
         <v>2234251</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -684,7 +719,7 @@
         <v>74250</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -706,7 +741,7 @@
         <v>86006</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -728,7 +763,7 @@
         <v>186221</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>4</v>
       </c>
@@ -750,7 +785,7 @@
         <v>759704</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>5</v>
       </c>
@@ -772,7 +807,7 @@
         <v>1217736</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>4</v>
       </c>
@@ -803,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>2</v>
       </c>
@@ -822,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>3</v>
       </c>
@@ -841,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -860,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -879,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>8</v>
       </c>
@@ -910,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>2</v>
       </c>
@@ -929,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>3</v>
       </c>
@@ -948,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>4</v>
       </c>
@@ -967,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>5</v>
       </c>
@@ -986,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>16</v>
       </c>
@@ -1005,7 +1040,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1053,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>3</v>
       </c>
@@ -1031,7 +1066,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1079,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>5</v>
       </c>
@@ -1057,13 +1092,13 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1123,7 @@
       </c>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="3">
         <v>1</v>
@@ -1108,7 +1143,7 @@
       </c>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
       <c r="C31" s="3">
         <v>1</v>
@@ -1125,7 +1160,7 @@
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
       <c r="C32" s="3">
         <v>2</v>
@@ -1142,7 +1177,7 @@
       </c>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
       <c r="C33" s="3">
         <v>2</v>
@@ -1159,7 +1194,7 @@
       </c>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
       <c r="C34" s="3">
         <v>2</v>
@@ -1176,7 +1211,7 @@
       </c>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
       <c r="C35" s="3">
         <v>4</v>
@@ -1193,7 +1228,7 @@
       </c>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
       <c r="C36" s="3">
         <v>4</v>
@@ -1210,7 +1245,7 @@
       </c>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
       <c r="C37" s="3">
         <v>4</v>
@@ -1227,7 +1262,7 @@
       </c>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
       <c r="C38" s="3">
         <v>8</v>
@@ -1244,7 +1279,7 @@
       </c>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
       <c r="C39" s="3">
         <v>8</v>
@@ -1261,7 +1296,7 @@
       </c>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
       <c r="C40" s="3">
         <v>8</v>
@@ -1278,7 +1313,7 @@
       </c>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
       <c r="C41" s="3">
         <v>16</v>
@@ -1295,7 +1330,7 @@
       </c>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
       <c r="C42" s="3">
         <v>16</v>
@@ -1312,7 +1347,7 @@
       </c>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
       <c r="C43" s="3">
         <v>16</v>
@@ -1329,14 +1364,14 @@
       </c>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45" s="3">
         <v>32</v>
       </c>
@@ -1354,7 +1389,7 @@
         <v>191873</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
       <c r="C46" s="3">
         <v>1</v>
@@ -1368,7 +1403,7 @@
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
       <c r="C47" s="3">
         <v>1</v>
@@ -1382,7 +1417,7 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B48" s="3"/>
       <c r="C48" s="3">
         <v>2</v>
@@ -1398,7 +1433,7 @@
         <v>94389</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
       <c r="C49" s="3">
         <v>2</v>
@@ -1414,7 +1449,7 @@
         <v>569795</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="3"/>
       <c r="C50" s="3">
         <v>2</v>
@@ -1428,7 +1463,7 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="3"/>
       <c r="C51" s="3">
         <v>4</v>
@@ -1444,7 +1479,7 @@
         <v>64169</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="3"/>
       <c r="C52" s="3">
         <v>4</v>
@@ -1460,7 +1495,7 @@
         <v>462611</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="3"/>
       <c r="C53" s="3">
         <v>4</v>
@@ -1476,7 +1511,7 @@
         <v>4149250</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="3"/>
       <c r="C54" s="3">
         <v>8</v>
@@ -1492,7 +1527,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="3"/>
       <c r="C55" s="3">
         <v>8</v>
@@ -1508,7 +1543,7 @@
         <v>269212</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="3"/>
       <c r="C56" s="3">
         <v>8</v>
@@ -1524,7 +1559,7 @@
         <v>1733102</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="3"/>
       <c r="C57" s="3">
         <v>16</v>
@@ -1540,7 +1575,7 @@
         <v>34626</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="3"/>
       <c r="C58" s="3">
         <v>16</v>
@@ -1556,7 +1591,7 @@
         <v>163825</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="3"/>
       <c r="C59" s="3">
         <v>16</v>
@@ -1572,14 +1607,14 @@
         <v>1417900</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="3">
         <v>8</v>
       </c>
@@ -1597,7 +1632,7 @@
         <v>79364</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
       <c r="C62" s="3">
         <v>1</v>
@@ -1613,7 +1648,7 @@
         <v>628021</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="3"/>
       <c r="C63" s="3">
         <v>1</v>
@@ -1629,7 +1664,7 @@
         <v>4751562</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
       <c r="C64" s="3">
         <v>2</v>
@@ -1645,7 +1680,7 @@
         <v>50565</v>
       </c>
     </row>
-    <row r="65" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
       <c r="C65" s="3">
         <v>2</v>
@@ -1661,7 +1696,7 @@
         <v>258526</v>
       </c>
     </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B66" s="3"/>
       <c r="C66" s="3">
         <v>2</v>
@@ -1677,7 +1712,7 @@
         <v>2469922</v>
       </c>
     </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B67" s="3"/>
       <c r="C67" s="3">
         <v>4</v>
@@ -1693,7 +1728,7 @@
         <v>37275</v>
       </c>
     </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B68" s="3"/>
       <c r="C68" s="3">
         <v>4</v>
@@ -1709,7 +1744,7 @@
         <v>183542</v>
       </c>
     </row>
-    <row r="69" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B69" s="3"/>
       <c r="C69" s="3">
         <v>4</v>
@@ -1725,7 +1760,7 @@
         <v>1513122</v>
       </c>
     </row>
-    <row r="70" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B70" s="3"/>
       <c r="C70" s="3">
         <v>8</v>
@@ -1741,7 +1776,7 @@
         <v>33971</v>
       </c>
     </row>
-    <row r="71" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B71" s="3"/>
       <c r="C71" s="3">
         <v>8</v>
@@ -1757,7 +1792,7 @@
         <v>128258</v>
       </c>
     </row>
-    <row r="72" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B72" s="3"/>
       <c r="C72" s="3">
         <v>8</v>
@@ -1773,7 +1808,7 @@
         <v>1140623</v>
       </c>
     </row>
-    <row r="73" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B73" s="3"/>
       <c r="C73" s="3">
         <v>16</v>
@@ -1789,7 +1824,7 @@
         <v>30118</v>
       </c>
     </row>
-    <row r="74" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B74" s="3"/>
       <c r="C74" s="3">
         <v>16</v>
@@ -1805,7 +1840,7 @@
         <v>127980</v>
       </c>
     </row>
-    <row r="75" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B75" s="3"/>
       <c r="C75" s="3">
         <v>16</v>
@@ -1824,7 +1859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B77" s="5" t="s">
         <v>13</v>
       </c>
@@ -1919,7 +1954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>1</v>
       </c>
@@ -2017,7 +2052,7 @@
         <v>34487</v>
       </c>
     </row>
-    <row r="79" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:36" x14ac:dyDescent="0.2">
       <c r="C79">
         <v>1</v>
       </c>
@@ -2097,7 +2132,7 @@
         <v>165247</v>
       </c>
     </row>
-    <row r="80" spans="2:36" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:36" x14ac:dyDescent="0.2">
       <c r="C80">
         <v>1</v>
       </c>
@@ -2177,7 +2212,7 @@
         <v>1279571</v>
       </c>
     </row>
-    <row r="81" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="81" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C81">
         <v>1</v>
       </c>
@@ -2257,7 +2292,7 @@
         <v>6054199</v>
       </c>
     </row>
-    <row r="82" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="82" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C82">
         <v>1</v>
       </c>
@@ -2337,7 +2372,7 @@
         <v>12203807</v>
       </c>
     </row>
-    <row r="83" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="83" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C83">
         <v>2</v>
       </c>
@@ -2417,7 +2452,7 @@
         <v>34105</v>
       </c>
     </row>
-    <row r="84" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="84" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C84">
         <v>2</v>
       </c>
@@ -2497,7 +2532,7 @@
         <v>118342</v>
       </c>
     </row>
-    <row r="85" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="85" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C85">
         <v>2</v>
       </c>
@@ -2577,7 +2612,7 @@
         <v>912313</v>
       </c>
     </row>
-    <row r="86" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="86" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C86">
         <v>2</v>
       </c>
@@ -2657,7 +2692,7 @@
         <v>4249302</v>
       </c>
     </row>
-    <row r="87" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="87" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C87">
         <v>2</v>
       </c>
@@ -2737,7 +2772,7 @@
         <v>6444961</v>
       </c>
     </row>
-    <row r="88" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="88" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C88">
         <v>4</v>
       </c>
@@ -2817,7 +2852,7 @@
         <v>29567</v>
       </c>
     </row>
-    <row r="89" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="89" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C89">
         <v>4</v>
       </c>
@@ -2897,7 +2932,7 @@
         <v>71982</v>
       </c>
     </row>
-    <row r="90" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="90" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C90">
         <v>4</v>
       </c>
@@ -2977,7 +3012,7 @@
         <v>523056</v>
       </c>
     </row>
-    <row r="91" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="91" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C91">
         <v>4</v>
       </c>
@@ -3057,7 +3092,7 @@
         <v>1900493</v>
       </c>
     </row>
-    <row r="92" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="92" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C92">
         <v>4</v>
       </c>
@@ -3137,7 +3172,7 @@
         <v>3897363</v>
       </c>
     </row>
-    <row r="93" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="93" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C93">
         <v>8</v>
       </c>
@@ -3217,7 +3252,7 @@
         <v>25522</v>
       </c>
     </row>
-    <row r="94" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="94" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C94">
         <v>8</v>
       </c>
@@ -3297,7 +3332,7 @@
         <v>65153</v>
       </c>
     </row>
-    <row r="95" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="95" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C95">
         <v>8</v>
       </c>
@@ -3377,7 +3412,7 @@
         <v>299233</v>
       </c>
     </row>
-    <row r="96" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="96" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C96">
         <v>8</v>
       </c>
@@ -3457,7 +3492,7 @@
         <v>1255730</v>
       </c>
     </row>
-    <row r="97" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="97" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C97">
         <v>8</v>
       </c>
@@ -3537,7 +3572,7 @@
         <v>1725723</v>
       </c>
     </row>
-    <row r="98" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="98" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C98">
         <v>16</v>
       </c>
@@ -3617,7 +3652,7 @@
         <v>22556</v>
       </c>
     </row>
-    <row r="99" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="99" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C99">
         <v>16</v>
       </c>
@@ -3697,7 +3732,7 @@
         <v>35476</v>
       </c>
     </row>
-    <row r="100" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="100" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C100">
         <v>16</v>
       </c>
@@ -3777,7 +3812,7 @@
         <v>163519</v>
       </c>
     </row>
-    <row r="101" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="101" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C101">
         <v>16</v>
       </c>
@@ -3857,7 +3892,7 @@
         <v>582960</v>
       </c>
     </row>
-    <row r="102" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="102" spans="3:36" x14ac:dyDescent="0.2">
       <c r="C102">
         <v>16</v>
       </c>
@@ -3937,7 +3972,7 @@
         <v>1018714</v>
       </c>
     </row>
-    <row r="105" spans="3:36" x14ac:dyDescent="0.4">
+    <row r="105" spans="3:36" x14ac:dyDescent="0.2">
       <c r="E105" t="s">
         <v>16</v>
       </c>
@@ -3946,4 +3981,1766 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE172F9-AE03-E846-9A45-1B22FCECC7E7}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>D2/60</f>
+        <v>22.024149583333333</v>
+      </c>
+      <c r="D2">
+        <f>E2/1000</f>
+        <v>1321.448975</v>
+      </c>
+      <c r="E2">
+        <v>1321448.9750000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C60" si="0">D3/60</f>
+        <v>21.818693950000004</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D60" si="1">E3/1000</f>
+        <v>1309.1216370000002</v>
+      </c>
+      <c r="E3">
+        <v>1309121.6370000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20.400293999999995</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>1224.0176399999998</v>
+      </c>
+      <c r="E4">
+        <v>1224017.6399999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>20.248072966666665</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1214.884378</v>
+      </c>
+      <c r="E5">
+        <v>1214884.378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>20.190021783333336</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1211.4013070000001</v>
+      </c>
+      <c r="E6">
+        <v>1211401.307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>20.245334616666664</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1214.7200769999999</v>
+      </c>
+      <c r="E7">
+        <v>1214720.077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>20.869180816666663</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1252.1508489999999</v>
+      </c>
+      <c r="E8">
+        <v>1252150.8489999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>11.273337983333333</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>676.40027899999995</v>
+      </c>
+      <c r="E9">
+        <v>676400.27899999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>11.449657666666667</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>686.97946000000002</v>
+      </c>
+      <c r="E10">
+        <v>686979.46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10.646157616666668</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>638.7694570000001</v>
+      </c>
+      <c r="E11">
+        <v>638769.45700000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10.2444173</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>614.66503799999998</v>
+      </c>
+      <c r="E12">
+        <v>614665.03799999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>11.934631483333332</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>716.07788899999991</v>
+      </c>
+      <c r="E13">
+        <v>716077.88899999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>22.773758366666666</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1366.4255020000001</v>
+      </c>
+      <c r="E14">
+        <v>1366425.5020000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>10.94101</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>656.4606</v>
+      </c>
+      <c r="E15">
+        <v>656460.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5.9837774833333324</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>359.02664899999996</v>
+      </c>
+      <c r="E16">
+        <v>359026.64899999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>6.3049625833333334</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>378.297755</v>
+      </c>
+      <c r="E17">
+        <v>378297.755</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>6.2861597333333332</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>377.16958399999999</v>
+      </c>
+      <c r="E18">
+        <v>377169.58399999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5.9084573666666662</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>354.50744199999997</v>
+      </c>
+      <c r="E19">
+        <v>354507.44199999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>18.785236816666668</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1127.1142090000001</v>
+      </c>
+      <c r="E20">
+        <v>1127114.209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>11.133000583333335</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>667.98003500000004</v>
+      </c>
+      <c r="E21">
+        <v>667980.03500000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5.3158866500000004</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>318.95319900000004</v>
+      </c>
+      <c r="E22">
+        <v>318953.19900000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.9028673999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>174.172044</v>
+      </c>
+      <c r="E23">
+        <v>174172.04399999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>3.1673898666666664</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>190.04339199999998</v>
+      </c>
+      <c r="E24">
+        <v>190043.39199999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>3.4294397333333331</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>205.76638399999999</v>
+      </c>
+      <c r="E25">
+        <v>205766.38399999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>19.146351799999998</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1148.7811079999999</v>
+      </c>
+      <c r="E26">
+        <v>1148781.108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>9.0843572833333344</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>545.06143700000007</v>
+      </c>
+      <c r="E27">
+        <v>545061.43700000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>5.1814205500000003</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>310.88523300000003</v>
+      </c>
+      <c r="E28">
+        <v>310885.23300000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>3.1841277333333333</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>191.047664</v>
+      </c>
+      <c r="E29">
+        <v>191047.66399999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1.62995935</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>97.797561000000002</v>
+      </c>
+      <c r="E30">
+        <v>97797.561000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1.9812450499999998</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>118.874703</v>
+      </c>
+      <c r="E31">
+        <v>118874.70299999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AEEC8D-9DB4-4F48-9BA4-FAEB46F1D9D2}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>D2/60</f>
+        <v>19.790500000000002</v>
+      </c>
+      <c r="D2">
+        <f>E2/1000</f>
+        <v>1187.43</v>
+      </c>
+      <c r="E2">
+        <v>1187430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C31" si="0">D3/60</f>
+        <v>19.471816666666665</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:E31" si="1">E3/1000</f>
+        <v>1168.309</v>
+      </c>
+      <c r="E3">
+        <v>1168309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>23.140616666666666</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>1388.4369999999999</v>
+      </c>
+      <c r="E4">
+        <v>1388437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>18.554766666666669</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1113.2860000000001</v>
+      </c>
+      <c r="E5">
+        <v>1113286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>18.424500000000002</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1105.47</v>
+      </c>
+      <c r="E6">
+        <v>1105470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>21.326183333333333</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1279.5709999999999</v>
+      </c>
+      <c r="E7">
+        <v>1279571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>19.619800000000001</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1177.1880000000001</v>
+      </c>
+      <c r="E8">
+        <v>1177188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>10.225416666666666</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>613.52499999999998</v>
+      </c>
+      <c r="E9">
+        <v>613525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>10.53965</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>632.37900000000002</v>
+      </c>
+      <c r="E10">
+        <v>632379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11.087166666666667</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>665.23</v>
+      </c>
+      <c r="E11">
+        <v>665230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10.152283333333333</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>609.13699999999994</v>
+      </c>
+      <c r="E12">
+        <v>609137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>15.205216666666667</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>912.31299999999999</v>
+      </c>
+      <c r="E13">
+        <v>912313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>17.815266666666666</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1068.9159999999999</v>
+      </c>
+      <c r="E14">
+        <v>1068916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>11.623850000000001</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>697.43100000000004</v>
+      </c>
+      <c r="E15">
+        <v>697431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5.5321499999999997</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>331.92899999999997</v>
+      </c>
+      <c r="E16">
+        <v>331929</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>5.8217666666666661</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>349.30599999999998</v>
+      </c>
+      <c r="E17">
+        <v>349306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>7.3052333333333337</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>438.31400000000002</v>
+      </c>
+      <c r="E18">
+        <v>438314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>8.7176000000000009</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>523.05600000000004</v>
+      </c>
+      <c r="E19">
+        <v>523056</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>19.476366666666667</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1168.5820000000001</v>
+      </c>
+      <c r="E20">
+        <v>1168582</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>9.85975</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>591.58500000000004</v>
+      </c>
+      <c r="E21">
+        <v>591585</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5.2438499999999992</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>314.63099999999997</v>
+      </c>
+      <c r="E22">
+        <v>314631</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.9014666666666664</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>174.08799999999999</v>
+      </c>
+      <c r="E23">
+        <v>174088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>3.6485500000000002</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>218.91300000000001</v>
+      </c>
+      <c r="E24">
+        <v>218913</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>4.9872166666666669</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>299.233</v>
+      </c>
+      <c r="E25">
+        <v>299233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>19.326566666666668</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1159.5940000000001</v>
+      </c>
+      <c r="E26">
+        <v>1159594</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>9.4018499999999996</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>564.11099999999999</v>
+      </c>
+      <c r="E27">
+        <v>564111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>4.9504166666666665</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>297.02499999999998</v>
+      </c>
+      <c r="E28">
+        <v>297025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2.8555833333333336</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>171.33500000000001</v>
+      </c>
+      <c r="E29">
+        <v>171335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1.6122833333333333</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>96.736999999999995</v>
+      </c>
+      <c r="E30">
+        <v>96737</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>2.7253166666666666</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>163.51900000000001</v>
+      </c>
+      <c r="E31">
+        <v>163519</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B375B171-EE6D-2447-B775-E9E85687C7E0}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>D2/60</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>E2/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C31" si="0">D3/60</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D31" si="1">E3/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4.7796333333333338</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>286.77800000000002</v>
+      </c>
+      <c r="E9">
+        <v>286778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3.6419333333333332</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>218.51599999999999</v>
+      </c>
+      <c r="E16">
+        <v>218516</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.8023000000000002</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>168.13800000000001</v>
+      </c>
+      <c r="E23">
+        <v>168138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2.3932500000000001</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>143.595</v>
+      </c>
+      <c r="E30">
+        <v>143595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>